<commit_message>
Solving issues between code version
</commit_message>
<xml_diff>
--- a/src/main/resources/panini-manga-titles.xlsx
+++ b/src/main/resources/panini-manga-titles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\IdeaProjects\batch-processing\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B0829C-0C2C-4D6F-8987-0E089B57FB7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB23600-A278-41D9-96FC-09A0FFA8421D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5663,7 +5663,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A288" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A325" sqref="A325:O326"/>
+      <selection pane="bottomLeft" activeCell="E327" sqref="E327"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Add titles and issues
</commit_message>
<xml_diff>
--- a/src/main/resources/panini-manga-titles.xlsx
+++ b/src/main/resources/panini-manga-titles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\IdeaProjects\batch-processing\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB23600-A278-41D9-96FC-09A0FFA8421D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934B73A5-1A6D-42BD-A385-1FD488EF0648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="panini-light-novels" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'panini-manga-titles'!$A$1:$P$326</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'panini-manga-titles'!$A$1:$P$328</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4384" uniqueCount="1579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4420" uniqueCount="1592">
   <si>
     <t>PUBLISHER</t>
   </si>
@@ -4774,6 +4774,45 @@
   </si>
   <si>
     <t>Overlord: Light Novel</t>
+  </si>
+  <si>
+    <t>There’s No Freaking Way I’ll Be Your Lover! Unless...</t>
+  </si>
+  <si>
+    <t>Romantic Comedy, Slice of Life, Yuri</t>
+  </si>
+  <si>
+    <t>Writer: Teren Mikami; Illustrator: Musshu</t>
+  </si>
+  <si>
+    <t>/ediciones/645475/theres_no_freaking_way_ill_be_your_lover_unless-rustica_con_sobrecubierta/todos</t>
+  </si>
+  <si>
+    <t>/catalogsearch/result/index/?collection=THERE´S+NO+FREAKING+WAY+I´LL+BE+YOUR+LOVER!+UNLESS&amp;q=there's&amp;product_list_order=name</t>
+  </si>
+  <si>
+    <t>Neon Genesis Evangelion: Collector's Edition</t>
+  </si>
+  <si>
+    <t>/ediciones/641196/neon_genesis_evangelion_-_collectors_edition-rustica_con_sobrecubierta/todos</t>
+  </si>
+  <si>
+    <t>/catalogsearch/result/index/?collection=EVANGELION+COLLECTOR'S+EDITION&amp;q=evangelion&amp;product_list_order=name</t>
+  </si>
+  <si>
+    <t>Mabataki yori Hayaku!!</t>
+  </si>
+  <si>
+    <t>Author: Kazuki Funatsu</t>
+  </si>
+  <si>
+    <t>Martial Arts, Sports</t>
+  </si>
+  <si>
+    <t>/ediciones/649017/mabataki_yori_hayaku-rustica_con_sobrecubierta/todos</t>
+  </si>
+  <si>
+    <t>/catalogsearch/result/index/?collection=MABATAKI+YORI+HAYAKU!!&amp;q=mabataki&amp;product_list_order=name</t>
   </si>
 </sst>
 </file>
@@ -5659,11 +5698,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P326"/>
+  <dimension ref="A1:P329"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A288" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E327" sqref="E327"/>
+      <pane ySplit="1" topLeftCell="A287" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L329" sqref="L329"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21798,7 +21837,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="321" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A321" s="3" t="s">
         <v>1013</v>
       </c>
@@ -21846,7 +21885,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="322" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A322" s="3" t="s">
         <v>1013</v>
       </c>
@@ -21894,7 +21933,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="323" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A323" s="3" t="s">
         <v>1013</v>
       </c>
@@ -21941,7 +21980,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="324" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A324" s="3" t="s">
         <v>1013</v>
       </c>
@@ -21989,7 +22028,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="325" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A325" s="3" t="s">
         <v>1013</v>
       </c>
@@ -22037,7 +22076,7 @@
         <v>1571</v>
       </c>
     </row>
-    <row r="326" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A326" s="3" t="s">
         <v>1013</v>
       </c>
@@ -22085,8 +22124,153 @@
         <v>1577</v>
       </c>
     </row>
+    <row r="327" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A327" s="3" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B327" s="3" t="s">
+        <v>1579</v>
+      </c>
+      <c r="C327" s="3" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(LOWER(B327)," ","-"),":",""),"'",""),"!",""),",",""),"é","e"),"'",""),".",""),"’","")</f>
+        <v>theres-no-freaking-way-ill-be-your-lover-unless</v>
+      </c>
+      <c r="D327" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E327" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F327" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G327" s="3" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H327" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I327" s="3" t="s">
+        <v>1001</v>
+      </c>
+      <c r="J327" s="3">
+        <v>5</v>
+      </c>
+      <c r="K327" s="1">
+        <v>45238</v>
+      </c>
+      <c r="L327" s="1" t="s">
+        <v>1580</v>
+      </c>
+      <c r="M327" s="1" t="s">
+        <v>1581</v>
+      </c>
+      <c r="N327" s="3" t="s">
+        <v>1582</v>
+      </c>
+      <c r="O327" s="3" t="s">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="328" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A328" s="3" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B328" s="5" t="s">
+        <v>1584</v>
+      </c>
+      <c r="C328" s="5" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(LOWER(B328)," ","-"),":",""),"'",""),"!",""),",",""),"é","e"),"'",""),".",""),"’","")</f>
+        <v>neon-genesis-evangelion-collectors-edition</v>
+      </c>
+      <c r="D328" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E328" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F328" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="G328" s="3" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H328" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I328" s="5" t="s">
+        <v>1001</v>
+      </c>
+      <c r="J328" s="5">
+        <v>7</v>
+      </c>
+      <c r="K328" s="6">
+        <v>45231</v>
+      </c>
+      <c r="L328" s="6" t="s">
+        <v>1205</v>
+      </c>
+      <c r="M328" s="6" t="s">
+        <v>1204</v>
+      </c>
+      <c r="N328" t="s">
+        <v>1585</v>
+      </c>
+      <c r="O328" s="7" t="s">
+        <v>1586</v>
+      </c>
+      <c r="P328" s="5"/>
+    </row>
+    <row r="329" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A329" s="3" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B329" s="3" t="s">
+        <v>1587</v>
+      </c>
+      <c r="C329" s="5" t="str">
+        <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(LOWER(B329)," ","-"),":",""),"'",""),"!",""),",",""),"é","e"),"'",""),".",""),"’","")</f>
+        <v>mabataki-yori-hayaku</v>
+      </c>
+      <c r="D329" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E329" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F329" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G329" s="3" t="s">
+        <v>1015</v>
+      </c>
+      <c r="H329" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I329" s="3" t="s">
+        <v>1001</v>
+      </c>
+      <c r="J329" s="3">
+        <v>9</v>
+      </c>
+      <c r="K329" s="1">
+        <v>45245</v>
+      </c>
+      <c r="L329" s="1" t="s">
+        <v>1589</v>
+      </c>
+      <c r="M329" s="1" t="s">
+        <v>1588</v>
+      </c>
+      <c r="N329" s="3" t="s">
+        <v>1590</v>
+      </c>
+      <c r="O329" s="3" t="s">
+        <v>1591</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:P326" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:P328" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>